<commit_message>
update export of delivery status, delivery type and return status; change the status of return
</commit_message>
<xml_diff>
--- a/backend/src/test/resources/excels/delivery_returns.xlsx
+++ b/backend/src/test/resources/excels/delivery_returns.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\projects\corgi-gift-delivery\backend\src\test\resources\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8B5FF5-C3C1-4A88-ACD7-50E9940067AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{4E8B5FF5-C3C1-4A88-ACD7-50E9940067AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB9A68D8-A9C0-40ED-9127-57C4682918A1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -33,41 +44,41 @@
     <t>customer_id</t>
   </si>
   <si>
+    <t>return_status</t>
+  </si>
+  <si>
     <t>note</t>
   </si>
   <si>
     <t>sn202508</t>
   </si>
   <si>
+    <t>YEU_CAU_TRA_HANG</t>
+  </si>
+  <si>
+    <t>Hàng bị lỗi</t>
+  </si>
+  <si>
+    <t>TIEP_NHAN_TRA_HANG</t>
+  </si>
+  <si>
+    <t>Hương xác nhận đồng ý nhận lại hàng</t>
+  </si>
+  <si>
     <t>sn202512</t>
   </si>
   <si>
-    <t>return_status</t>
-  </si>
-  <si>
-    <t>YEU_CAU_TRA_HANG</t>
-  </si>
-  <si>
-    <t>Hàng bị lỗi</t>
-  </si>
-  <si>
-    <t>NCC_DA_NHAN_TRA_HANG</t>
-  </si>
-  <si>
-    <t>Viettien đã đồng ý hoàn hàng</t>
-  </si>
-  <si>
-    <t>NCC_DA_DOI_HANG</t>
-  </si>
-  <si>
-    <t>Katinat đã đổi lý mới cho anh H</t>
+    <t>DA_TRA_HANG</t>
+  </si>
+  <si>
+    <t>Hương đã nhận trả hàng thành công</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,18 +87,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -133,12 +149,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,70 +438,70 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="4">
         <v>321891</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>321903</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>321903</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>321895</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>